<commit_message>
Changes - new rewards
</commit_message>
<xml_diff>
--- a/reward-graph-curve-fitter.xlsx
+++ b/reward-graph-curve-fitter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.d.srinivas\Desktop\repos\Personal\deepracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982808BF-7543-4D79-AE45-A8AED5A0EA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55327BAC-1463-432C-AAE9-DC4515982C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E4E61E1-599E-4A85-97CA-52F2C3418F7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Speed</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Steering Angle</t>
+  </si>
+  <si>
+    <t>distance</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D9AF17-2F82-47FD-BCB9-3B557DA993B6}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="A28" sqref="A28:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +731,51 @@
         <v>50</v>
       </c>
     </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.05</v>
+      </c>
+      <c r="B29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.1</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.3</v>
+      </c>
+      <c r="B31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>